<commit_message>
Update admission automation (login to submit admission)
</commit_message>
<xml_diff>
--- a/excel/admission.xlsx
+++ b/excel/admission.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="163">
   <si>
     <t>Xpath</t>
   </si>
@@ -48,9 +48,6 @@
     <t>click</t>
   </si>
   <si>
-    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/div[2]/div/div/div[1]/button[2]</t>
-  </si>
-  <si>
     <t>New Patient</t>
   </si>
   <si>
@@ -60,57 +57,24 @@
     <t>visible</t>
   </si>
   <si>
-    <t>//*[@id="input_341"]</t>
-  </si>
-  <si>
-    <t>//*[@id="input_342"]</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
-    <t>//*[@id="dialogContent_339"]</t>
-  </si>
-  <si>
-    <t>//*[@id="input_343"]</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>//*[@id="select_346"]</t>
-  </si>
-  <si>
-    <t>//*[@id="select_option_344"]</t>
-  </si>
-  <si>
-    <t>//*[@id="dialogContent_339"]/div[2]/div[1]/div[1]/form/div/md-datepicker/div[1]/input</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>input</t>
   </si>
   <si>
-    <t>//*[@id="dialogContent_339"]/div[2]/div[1]/div[2]/button[3]</t>
-  </si>
-  <si>
     <t>Confirm Button</t>
   </si>
   <si>
-    <t>Edward</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -144,23 +108,422 @@
     <t>password</t>
   </si>
   <si>
-    <t>Delay Before Action(Minute)</t>
-  </si>
-  <si>
-    <t>Delay After Action(Minute)</t>
+    <t>Delay Before Action(Sec)</t>
+  </si>
+  <si>
+    <t>Delay After Action(Sec)</t>
+  </si>
+  <si>
+    <t>(//button[@type='button'])[76]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_15"]</t>
+  </si>
+  <si>
+    <t>//*[@id="dialogContent_13"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_16"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_17"]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_20"]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_18"]</t>
+  </si>
+  <si>
+    <t>Gender Select</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>//*[@id="dialogContent_13"]/div[2]/div[1]/div[1]/form/div/md-datepicker/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="dialogContent_13"]/div[2]/div[1]/div[2]/button[3]</t>
+  </si>
+  <si>
+    <t>03-10-2017</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/md-list/md-list-item[1]/div/button</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Intake Panel</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Approval Info Panel</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-actions/button</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[1]/md-content/form/div/md-datepicker/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="input_39"]</t>
+  </si>
+  <si>
+    <t>Medical Record Number</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_42"]</t>
+  </si>
+  <si>
+    <t>Transfer Status Assigned</t>
+  </si>
+  <si>
+    <t>//*[@id="select_45"]</t>
+  </si>
+  <si>
+    <t>Kaiser Transfer</t>
+  </si>
+  <si>
+    <t>//*[@id="fl-input-47"]</t>
+  </si>
+  <si>
+    <t>Approving Manager</t>
+  </si>
+  <si>
+    <t>//*[@id="ul-47"]/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="fl-input-48"]</t>
+  </si>
+  <si>
+    <t>Admitting Clinician Assigned</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_49"]</t>
+  </si>
+  <si>
+    <t>Patient Discharge Status</t>
+  </si>
+  <si>
+    <t>Select Patient Discharge Status</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_56"]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_58"]</t>
+  </si>
+  <si>
+    <t>Special Program</t>
+  </si>
+  <si>
+    <t>Select Special Program</t>
+  </si>
+  <si>
+    <t>Physician and Insurance Info</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[1]/md-card[1]/md-card-actions/button</t>
+  </si>
+  <si>
+    <t>Edit Primary Physicians</t>
+  </si>
+  <si>
+    <t>//*[@id="fl-input-65"]</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>//*[@id="ul-65"]/li[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_66"]</t>
+  </si>
+  <si>
+    <t>Primary Physician</t>
+  </si>
+  <si>
+    <t>Select Primary physician</t>
+  </si>
+  <si>
+    <t>Successfully Verified</t>
+  </si>
+  <si>
+    <t>Select Verified</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[3]/md-content/form/button</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[1]/md-content/button</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[2]/span[2]</t>
+  </si>
+  <si>
+    <t>Referral Date</t>
+  </si>
+  <si>
+    <t>match_text</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[3]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[4]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[5]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[6]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-expanded/md-expansion-panel-content/div/md-card/md-card-content/div[7]/span[2]</t>
+  </si>
+  <si>
+    <t>Mar 10, 2017</t>
+  </si>
+  <si>
+    <t>Jenny, Duque</t>
+  </si>
+  <si>
+    <t>Jennifer, Cortez</t>
+  </si>
+  <si>
+    <t>Patient is at Home</t>
+  </si>
+  <si>
+    <t>SNP, Same Day Joints</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[1]/md-card[1]/md-card-content[1]/span[1]</t>
+  </si>
+  <si>
+    <t>Hamoudi, Al Bander</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[1]/md-card[1]/md-card-content[1]/span[3]/span[1]</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>02-02-2017</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-actions/button</t>
+  </si>
+  <si>
+    <t>Insurance Infor Edit</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[5]/md-content/form/div/md-datepicker/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="fl-input-76"]</t>
+  </si>
+  <si>
+    <t>ngs</t>
+  </si>
+  <si>
+    <t>//*[@id="ul-76"]/li</t>
+  </si>
+  <si>
+    <t>Primary Insurance</t>
+  </si>
+  <si>
+    <t>Select Primary Insurance</t>
+  </si>
+  <si>
+    <t>//*[@id="input_77"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_78"]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_81"]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_option_79"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_83"]</t>
+  </si>
+  <si>
+    <t>7955125</t>
+  </si>
+  <si>
+    <t>5465225</t>
+  </si>
+  <si>
+    <t>313</t>
+  </si>
+  <si>
+    <t>HIC Number</t>
+  </si>
+  <si>
+    <t>Primary Policy Number</t>
+  </si>
+  <si>
+    <t>Verification Printed and Filed</t>
+  </si>
+  <si>
+    <t>Insurance Authorization Code</t>
+  </si>
+  <si>
+    <t>Select Verification printed Field</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[5]/md-content/button</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[2]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[3]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[4]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[5]/span[2]/span[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[1]/md-card-content/div[6]/span[2]</t>
+  </si>
+  <si>
+    <t>Soc Date</t>
+  </si>
+  <si>
+    <t>Feb 2, 2017</t>
+  </si>
+  <si>
+    <t>NGS</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[2]/md-card-actions/button</t>
+  </si>
+  <si>
+    <t>Pre-auth Info</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-sidenav[6]/md-content/button</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>OT</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[2]/md-card-content/div[1]/span[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[2]/md-card-content/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[2]/md-card[2]/md-card-content/div[1]/span[3]</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>//div[@id='widget']/div/div/md-list/md-list-item/div/div/h4</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[1]/md-expansion-panel-collapsed/md-icon</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-collapsed/md-icon</t>
+  </si>
+  <si>
+    <t>//*[@id="ul-48"]/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="select_53"]</t>
+  </si>
+  <si>
+    <t>Select first</t>
+  </si>
+  <si>
+    <t>Select First</t>
+  </si>
+  <si>
+    <t>Duque</t>
+  </si>
+  <si>
+    <t>Cortez</t>
+  </si>
+  <si>
+    <t>//*[@id="select_60"]</t>
+  </si>
+  <si>
+    <t>/html/body/md-backdrop</t>
+  </si>
+  <si>
+    <t>clcose background</t>
+  </si>
+  <si>
+    <t>//*[@id="select_68"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_84"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_85"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_86"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-actions/button[2]</t>
+  </si>
+  <si>
+    <t>Submit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,13 +546,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,7 +856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -495,10 +866,12 @@
   <cols>
     <col min="1" max="1" width="24.7109375" style="1"/>
     <col min="2" max="2" width="53.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="24.7109375" style="1"/>
+    <col min="3" max="3" width="24.7109375" style="1"/>
+    <col min="4" max="4" width="24.7109375" style="2"/>
+    <col min="5" max="16384" width="24.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -508,53 +881,71 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="48.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -571,10 +962,10 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -629,12 +1020,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -643,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -651,63 +1042,99 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -723,8 +1150,11 @@
       </c>
     </row>
     <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -741,16 +1171,16 @@
     </row>
     <row r="15" spans="1:7" ht="30">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="2">
-        <v>42767</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -764,10 +1194,10 @@
     </row>
     <row r="16" spans="1:7" ht="30">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -779,6 +1209,1272 @@
         <v>1</v>
       </c>
       <c r="G16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="75">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30">
+      <c r="A35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="75">
+      <c r="A36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="75">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="75">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="75">
+      <c r="A39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="75">
+      <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="75">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="75">
+      <c r="A42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30">
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="75">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30">
+      <c r="A49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="75">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="90">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="75">
+      <c r="A52" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45">
+      <c r="A53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30">
+      <c r="A59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30">
+      <c r="A61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="90">
+      <c r="A62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="90">
+      <c r="A63" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="90">
+      <c r="A64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="90">
+      <c r="A65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="90">
+      <c r="A66" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="90">
+      <c r="A67" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D67" s="4">
+        <v>123123</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="75">
+      <c r="A68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="30">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="90">
+      <c r="A73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="90">
+      <c r="A74" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="90">
+      <c r="A75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30">
+      <c r="A76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>